<commit_message>
adding just wallops as GS option
</commit_message>
<xml_diff>
--- a/Scenarios/parameters_gs_network.xlsx
+++ b/Scenarios/parameters_gs_network.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="16060" tabRatio="500" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="2980" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="sim_parameters" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <sheet name="4" sheetId="12" r:id="rId9"/>
     <sheet name="5" sheetId="13" r:id="rId10"/>
     <sheet name="6" sheetId="14" r:id="rId11"/>
-    <sheet name="gs_generator" sheetId="11" r:id="rId12"/>
+    <sheet name="7" sheetId="16" r:id="rId12"/>
+    <sheet name="8" sheetId="17" r:id="rId13"/>
+    <sheet name="gs_generator" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -360,6 +362,15 @@
   </si>
   <si>
     <t>Equatorial alternative</t>
+  </si>
+  <si>
+    <t>avail. From my own analysis (col E is with mix of Inigo's and my numbers)</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>Wallops</t>
   </si>
 </sst>
 </file>
@@ -442,8 +453,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -551,7 +572,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -594,6 +615,11 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -636,6 +662,11 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1194,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1205,7 +1236,7 @@
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1224,8 +1255,11 @@
       <c r="F1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="J1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1239,13 +1273,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="12">
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="J2" s="12">
+        <v>0.28220000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1259,13 +1296,16 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.49</v>
       </c>
       <c r="F3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="J3">
+        <v>0.16370000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1279,13 +1319,16 @@
         <v>0</v>
       </c>
       <c r="E4" s="12">
-        <v>1</v>
+        <v>0.59809999999999997</v>
       </c>
       <c r="F4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="J4" s="12">
+        <v>0.59809999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1299,13 +1342,16 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.15329999999999999</v>
       </c>
       <c r="F5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="J5">
+        <v>0.15329999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1319,13 +1365,16 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.20369999999999999</v>
       </c>
       <c r="F6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="J6">
+        <v>0.20369999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1339,13 +1388,16 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.60840000000000005</v>
       </c>
       <c r="F7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="J7">
+        <v>0.60840000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1359,13 +1411,16 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.65439999999999998</v>
       </c>
       <c r="F8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="J8">
+        <v>0.65439999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1379,13 +1434,16 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.8448</v>
       </c>
       <c r="F9" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="J9">
+        <v>0.8448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1399,13 +1457,16 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.74280000000000002</v>
       </c>
       <c r="F10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="16">
+      <c r="J10">
+        <v>0.74280000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16">
       <c r="D16" s="13"/>
     </row>
   </sheetData>
@@ -1421,10 +1482,186 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>37.855662000000002</v>
+      </c>
+      <c r="C2" s="12">
+        <v>-75.512068999999997</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>42.360726</v>
+      </c>
+      <c r="C3">
+        <v>-71.093208000000004</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="E4" s="12"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="D6" s="12"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="D10" s="12"/>
+    </row>
+    <row r="16" spans="1:10" ht="16">
+      <c r="D16" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>37.855662000000002</v>
+      </c>
+      <c r="C2" s="12">
+        <v>-75.512068999999997</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="E4" s="12"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="D6" s="12"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="D10" s="12"/>
+    </row>
+    <row r="16" spans="1:10" ht="16">
+      <c r="D16" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2278,7 +2515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2382,7 +2619,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3476,7 +3713,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updates to single sat generator
</commit_message>
<xml_diff>
--- a/Scenarios/parameters_gs_network.xlsx
+++ b/Scenarios/parameters_gs_network.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="2980" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="6" sheetId="14" r:id="rId8"/>
     <sheet name="7" sheetId="16" r:id="rId9"/>
     <sheet name="8" sheetId="17" r:id="rId10"/>
-    <sheet name="gs_generator" sheetId="11" r:id="rId11"/>
+    <sheet name="9" sheetId="18" r:id="rId11"/>
+    <sheet name="gs_generator" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -287,6 +288,12 @@
   </si>
   <si>
     <t>czml_content.append(cztl.createGS('</t>
+  </si>
+  <si>
+    <t>SFN_antarctica</t>
+  </si>
+  <si>
+    <t>Antarctica 17</t>
   </si>
 </sst>
 </file>
@@ -361,8 +368,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -500,7 +509,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="121">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -560,6 +569,7 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -619,6 +629,7 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -956,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1061,6 +1072,14 @@
       </c>
       <c r="B10" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1153,9 +1172,410 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>70.366209999999995</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-148.745529</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>64.836530999999994</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-147.65174500000001</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>47.606000000000002</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-122.33</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>32.787199999999999</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-106.3257</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42.942349999999998</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-71.636094999999997</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>19.896799999999999</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-155.58279999999999</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>26.754200000000001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-80.933700000000002</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-53.163800000000002</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-70.917100000000005</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-18.415921000000001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-45.633626999999997</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>48.135100000000001</v>
+      </c>
+      <c r="C11" s="1">
+        <v>11.582000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>67.316000000000003</v>
+      </c>
+      <c r="C12" s="1">
+        <v>14.776999999999999</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-25.89</v>
+      </c>
+      <c r="C13" s="1">
+        <v>27.685300000000002</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>25.204799999999999</v>
+      </c>
+      <c r="C14" s="1">
+        <v>55.270800000000001</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.3521000000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>103.8198</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>13.4443</v>
+      </c>
+      <c r="C16" s="1">
+        <v>144.7937</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>37.516871000000002</v>
+      </c>
+      <c r="C17" s="1">
+        <v>139.66645399999999</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>-46.512945000000002</v>
+      </c>
+      <c r="C18" s="1">
+        <v>168.37595200000001</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>-72</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding updated gs params file, as well as scenario for tundra orbit
</commit_message>
<xml_diff>
--- a/Scenarios/parameters_gs_network.xlsx
+++ b/Scenarios/parameters_gs_network.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="2980" yWindow="0" windowWidth="29580" windowHeight="16380" tabRatio="500" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -293,7 +293,7 @@
     <t>SFN_antarctica</t>
   </si>
   <si>
-    <t>Antarctica 17</t>
+    <t>Antarctica 18</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1175,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
more updates to params file, was mistaken before
</commit_message>
<xml_diff>
--- a/Scenarios/parameters_gs_network.xlsx
+++ b/Scenarios/parameters_gs_network.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="0" windowWidth="29580" windowHeight="16380" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="19080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <sheet name="7" sheetId="16" r:id="rId9"/>
     <sheet name="8" sheetId="17" r:id="rId10"/>
     <sheet name="9" sheetId="18" r:id="rId11"/>
-    <sheet name="gs_generator" sheetId="11" r:id="rId12"/>
+    <sheet name="10" sheetId="19" r:id="rId12"/>
+    <sheet name="11" sheetId="20" r:id="rId13"/>
+    <sheet name="gs_generator" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -290,10 +292,64 @@
     <t>czml_content.append(cztl.createGS('</t>
   </si>
   <si>
+    <t>0C isotherm Height (km)</t>
+  </si>
+  <si>
+    <t>Map region letter</t>
+  </si>
+  <si>
+    <t>1% exceeded rain rate</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Antarctica 18</t>
+  </si>
+  <si>
+    <t>KSAT equatorial</t>
+  </si>
+  <si>
+    <t>1, Ka</t>
+  </si>
+  <si>
+    <t>Only those ground stations from the KSAT network that lie near the equator</t>
+  </si>
+  <si>
+    <t>singapore</t>
+  </si>
+  <si>
     <t>SFN_antarctica</t>
-  </si>
-  <si>
-    <t>Antarctica 18</t>
   </si>
 </sst>
 </file>
@@ -306,6 +362,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -368,10 +425,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="121">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -509,7 +564,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="121">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -569,7 +624,6 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -629,7 +683,6 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -967,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -979,7 +1032,7 @@
     <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -990,7 +1043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1001,7 +1054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1012,7 +1065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1023,7 +1076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1034,7 +1087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1042,7 +1095,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1050,7 +1103,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1058,7 +1111,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1066,7 +1119,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1074,13 +1127,39 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
+    <row r="11" spans="1:4">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
+      <c r="B11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1097,7 +1176,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1172,15 +1251,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1270,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -1199,370 +1278,561 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>70.366209999999995</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-148.745529</v>
+      <c r="B2" s="2">
+        <v>68.360699999999994</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-133.72300000000001</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>64.836530999999994</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-147.65174500000001</v>
+      <c r="B3" s="2">
+        <v>64.837800000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-147.71639999999999</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>47.606000000000002</v>
-      </c>
-      <c r="C4" s="1">
-        <v>-122.33</v>
+      <c r="B4" s="2">
+        <v>35.272561099999997</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-120.7054055</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>32.787199999999999</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-106.3257</v>
+      <c r="B5" s="2">
+        <v>20.72</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-156.26</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>42.942349999999998</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-71.636094999999997</v>
+      <c r="B6" s="2">
+        <v>8.5380000000000003</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-80.7821</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>19.896799999999999</v>
-      </c>
-      <c r="C7" s="1">
-        <v>-155.58279999999999</v>
+      <c r="B7" s="3">
+        <v>-31.420100000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-64.188800000000001</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <v>26.754200000000001</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-80.933700000000002</v>
+      <c r="B8" s="2">
+        <v>-53.7790629</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-67.773556900000003</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>-53.163800000000002</v>
-      </c>
-      <c r="C9" s="1">
-        <v>-70.917100000000005</v>
+      <c r="B9" s="2">
+        <v>77.875</v>
+      </c>
+      <c r="C9" s="2">
+        <v>20.975200000000001</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
-        <v>-18.415921000000001</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-45.633626999999997</v>
+      <c r="B10" s="5">
+        <v>70.370599999999996</v>
+      </c>
+      <c r="C10" s="2">
+        <v>31.109400000000001</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>48.135100000000001</v>
-      </c>
-      <c r="C11" s="1">
-        <v>11.582000000000001</v>
+      <c r="B11" s="2">
+        <v>69.649199999999993</v>
+      </c>
+      <c r="C11" s="2">
+        <v>18.955300000000001</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>67.316000000000003</v>
-      </c>
-      <c r="C12" s="1">
-        <v>14.776999999999999</v>
+      <c r="B12" s="2">
+        <v>58.344700000000003</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8.5949000000000009</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
-        <v>-25.89</v>
-      </c>
-      <c r="C13" s="1">
-        <v>27.685300000000002</v>
+      <c r="B13" s="2">
+        <v>40.463700000000003</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-3.7492000000000001</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="F13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
-        <v>25.204799999999999</v>
-      </c>
-      <c r="C14" s="1">
-        <v>55.270800000000001</v>
+      <c r="B14" s="2">
+        <v>37.741199999999999</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-25.675599999999999</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
-        <v>1.3521000000000001</v>
-      </c>
-      <c r="C15" s="1">
-        <v>103.8198</v>
+      <c r="B15" s="2">
+        <v>4.5206189999999999</v>
+      </c>
+      <c r="C15" s="2">
+        <v>9.7497520000000009</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
-        <v>13.4443</v>
-      </c>
-      <c r="C16" s="1">
-        <v>144.7937</v>
+      <c r="B16" s="2">
+        <v>-25.64</v>
+      </c>
+      <c r="C16" s="2">
+        <v>28.08</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="F16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
-        <v>37.516871000000002</v>
-      </c>
-      <c r="C17" s="1">
-        <v>139.66645399999999</v>
+      <c r="B17" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>55.27</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="F17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
-        <v>-46.512945000000002</v>
-      </c>
-      <c r="C18" s="1">
-        <v>168.37595200000001</v>
+      <c r="B18" s="3">
+        <v>-20.348400000000002</v>
+      </c>
+      <c r="C18" s="2">
+        <v>57.552199999999999</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="F18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
-        <v>-72</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2</v>
+      <c r="B19" s="2">
+        <v>12.9716</v>
+      </c>
+      <c r="C19" s="2">
+        <v>77.5946</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
-        <v>87</v>
+      <c r="F19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.3521000000000001</v>
+      </c>
+      <c r="C20" s="2">
+        <v>103.8198</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>35.689500000000002</v>
+      </c>
+      <c r="C21" s="2">
+        <v>139.6917</v>
+      </c>
+      <c r="D21">
+        <v>4.5</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>-40.900599999999997</v>
+      </c>
+      <c r="C22" s="2">
+        <v>174.886</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1573,10 +1843,476 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1.3309905</v>
+      </c>
+      <c r="C2" s="8">
+        <v>103.8024025</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="8">
+        <v>2022</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>70.366209999999995</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-148.745529</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>64.836530999999994</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-147.65174500000001</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>47.606000000000002</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-122.33</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>32.787199999999999</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-106.3257</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42.942349999999998</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-71.636094999999997</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>19.896799999999999</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-155.58279999999999</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>26.754200000000001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-80.933700000000002</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-53.163800000000002</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-70.917100000000005</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-18.415921000000001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-45.633626999999997</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>48.135100000000001</v>
+      </c>
+      <c r="C11" s="1">
+        <v>11.582000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>67.316000000000003</v>
+      </c>
+      <c r="C12" s="1">
+        <v>14.776999999999999</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-25.89</v>
+      </c>
+      <c r="C13" s="1">
+        <v>27.685300000000002</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>25.204799999999999</v>
+      </c>
+      <c r="C14" s="1">
+        <v>55.270800000000001</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.3521000000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>103.8198</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>13.4443</v>
+      </c>
+      <c r="C16" s="1">
+        <v>144.7937</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>37.516871000000002</v>
+      </c>
+      <c r="C17" s="1">
+        <v>139.66645399999999</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>-46.512945000000002</v>
+      </c>
+      <c r="C18" s="1">
+        <v>168.37595200000001</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>-72</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updates to KSAT in gs params worksheet, and also walker generator wrapper has tiny changes
</commit_message>
<xml_diff>
--- a/Scenarios/parameters_gs_network.xlsx
+++ b/Scenarios/parameters_gs_network.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -337,19 +337,16 @@
     <t>Antarctica 18</t>
   </si>
   <si>
-    <t>KSAT equatorial</t>
-  </si>
-  <si>
-    <t>1, Ka</t>
-  </si>
-  <si>
-    <t>Only those ground stations from the KSAT network that lie near the equator</t>
-  </si>
-  <si>
     <t>singapore</t>
   </si>
   <si>
     <t>SFN_antarctica</t>
+  </si>
+  <si>
+    <t>KSAT (more detail?)</t>
+  </si>
+  <si>
+    <t>Note: for KSAT equatorial, just add the non-desired ground stations to the ignore list</t>
   </si>
 </sst>
 </file>
@@ -362,7 +359,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -425,8 +421,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -564,7 +562,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="121">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -624,6 +622,7 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -683,6 +682,7 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1020,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1032,7 +1032,7 @@
     <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1075,8 +1075,11 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1127,42 +1130,39 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="8">
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
crap, screwed up gs_network=11 in params_gs_network doc - used the SFN ground stations in it instead of KSAT. Updating that now to be the original 21 KSAT GS + Antarctica
</commit_message>
<xml_diff>
--- a/Scenarios/parameters_gs_network.xlsx
+++ b/Scenarios/parameters_gs_network.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="19080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="19080" tabRatio="500" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -337,16 +337,19 @@
     <t>Antarctica 18</t>
   </si>
   <si>
+    <t>KSAT equatorial</t>
+  </si>
+  <si>
+    <t>1, Ka</t>
+  </si>
+  <si>
+    <t>Only those ground stations from the KSAT network that lie near the equator</t>
+  </si>
+  <si>
     <t>singapore</t>
   </si>
   <si>
     <t>SFN_antarctica</t>
-  </si>
-  <si>
-    <t>KSAT (more detail?)</t>
-  </si>
-  <si>
-    <t>Note: for KSAT equatorial, just add the non-desired ground stations to the ignore list</t>
   </si>
 </sst>
 </file>
@@ -421,8 +424,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="121">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -562,7 +573,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="121">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -623,6 +634,10 @@
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -683,6 +698,10 @@
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1020,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1032,7 +1051,7 @@
     <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -1043,7 +1062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1054,7 +1073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1065,7 +1084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1075,11 +1094,8 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1090,7 +1106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1098,7 +1114,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1106,7 +1122,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1114,7 +1130,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1122,7 +1138,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1130,39 +1146,42 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:4">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:5">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="8">
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:4">
       <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1833,6 +1852,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1909,15 +1929,18 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1951,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -1936,369 +1959,588 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>70.366209999999995</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-148.745529</v>
+      <c r="B2" s="2">
+        <v>68.360699999999994</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-133.72300000000001</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>64.836530999999994</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-147.65174500000001</v>
+      <c r="B3" s="2">
+        <v>64.837800000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-147.71639999999999</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>47.606000000000002</v>
-      </c>
-      <c r="C4" s="1">
-        <v>-122.33</v>
+      <c r="B4" s="2">
+        <v>35.272561099999997</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-120.7054055</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>32.787199999999999</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-106.3257</v>
+      <c r="B5" s="2">
+        <v>20.72</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-156.26</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>42.942349999999998</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-71.636094999999997</v>
+      <c r="B6" s="2">
+        <v>8.5380000000000003</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-80.7821</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>19.896799999999999</v>
-      </c>
-      <c r="C7" s="1">
-        <v>-155.58279999999999</v>
+      <c r="B7" s="3">
+        <v>-31.420100000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-64.188800000000001</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <v>26.754200000000001</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-80.933700000000002</v>
+      <c r="B8" s="2">
+        <v>-53.7790629</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-67.773556900000003</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>-53.163800000000002</v>
-      </c>
-      <c r="C9" s="1">
-        <v>-70.917100000000005</v>
+      <c r="B9" s="2">
+        <v>77.875</v>
+      </c>
+      <c r="C9" s="2">
+        <v>20.975200000000001</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
-        <v>-18.415921000000001</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-45.633626999999997</v>
+      <c r="B10" s="5">
+        <v>70.370599999999996</v>
+      </c>
+      <c r="C10" s="2">
+        <v>31.109400000000001</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>48.135100000000001</v>
-      </c>
-      <c r="C11" s="1">
-        <v>11.582000000000001</v>
+      <c r="B11" s="2">
+        <v>69.649199999999993</v>
+      </c>
+      <c r="C11" s="2">
+        <v>18.955300000000001</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>67.316000000000003</v>
-      </c>
-      <c r="C12" s="1">
-        <v>14.776999999999999</v>
+      <c r="B12" s="2">
+        <v>58.344700000000003</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8.5949000000000009</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
-        <v>-25.89</v>
-      </c>
-      <c r="C13" s="1">
-        <v>27.685300000000002</v>
+      <c r="B13" s="2">
+        <v>40.463700000000003</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-3.7492000000000001</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="F13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
-        <v>25.204799999999999</v>
-      </c>
-      <c r="C14" s="1">
-        <v>55.270800000000001</v>
+      <c r="B14" s="2">
+        <v>37.741199999999999</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-25.675599999999999</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
-        <v>1.3521000000000001</v>
-      </c>
-      <c r="C15" s="1">
-        <v>103.8198</v>
+      <c r="B15" s="2">
+        <v>4.5206189999999999</v>
+      </c>
+      <c r="C15" s="2">
+        <v>9.7497520000000009</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
-        <v>13.4443</v>
-      </c>
-      <c r="C16" s="1">
-        <v>144.7937</v>
+      <c r="B16" s="2">
+        <v>-25.64</v>
+      </c>
+      <c r="C16" s="2">
+        <v>28.08</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="F16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
-        <v>37.516871000000002</v>
-      </c>
-      <c r="C17" s="1">
-        <v>139.66645399999999</v>
+      <c r="B17" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>55.27</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="F17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
-        <v>-46.512945000000002</v>
-      </c>
-      <c r="C18" s="1">
-        <v>168.37595200000001</v>
+      <c r="B18" s="3">
+        <v>-20.348400000000002</v>
+      </c>
+      <c r="C18" s="2">
+        <v>57.552199999999999</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="F18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
+        <v>12.9716</v>
+      </c>
+      <c r="C19" s="2">
+        <v>77.5946</v>
+      </c>
+      <c r="D19">
+        <v>5.5</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.3521000000000001</v>
+      </c>
+      <c r="C20" s="2">
+        <v>103.8198</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>35.689500000000002</v>
+      </c>
+      <c r="C21" s="2">
+        <v>139.6917</v>
+      </c>
+      <c r="D21">
+        <v>4.5</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>-40.900599999999997</v>
+      </c>
+      <c r="C22" s="2">
+        <v>174.886</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
         <v>-72</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C23" s="1">
         <v>2</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
         <v>100</v>
+      </c>
+      <c r="G23" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2984,7 +3226,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="F18" sqref="A2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3362,10 +3604,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="H22" sqref="A1:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3373,7 +3615,7 @@
     <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3384,7 +3626,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -3392,8 +3634,14 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16">
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3404,7 +3652,7 @@
         <v>-133.72300000000001</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3412,8 +3660,14 @@
       <c r="F2" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="16">
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3424,7 +3678,7 @@
         <v>-147.71639999999999</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3432,8 +3686,14 @@
       <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="16">
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3444,7 +3704,7 @@
         <v>-120.7054055</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3452,8 +3712,14 @@
       <c r="F4" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="16">
+      <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3464,7 +3730,7 @@
         <v>-156.26</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3472,8 +3738,14 @@
       <c r="F5" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="16">
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3484,7 +3756,7 @@
         <v>-80.7821</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3492,8 +3764,14 @@
       <c r="F6" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="16">
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3504,7 +3782,7 @@
         <v>-64.188800000000001</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3512,8 +3790,14 @@
       <c r="F7" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="16">
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3524,7 +3808,7 @@
         <v>-67.773556900000003</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3532,8 +3816,14 @@
       <c r="F8" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="16">
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3544,7 +3834,7 @@
         <v>20.975200000000001</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -3552,8 +3842,14 @@
       <c r="F9" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="16">
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3564,7 +3860,7 @@
         <v>31.109400000000001</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -3572,8 +3868,14 @@
       <c r="F10" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="16">
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3584,7 +3886,7 @@
         <v>18.955300000000001</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -3592,8 +3894,14 @@
       <c r="F11" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="16">
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3604,7 +3912,7 @@
         <v>8.5949000000000009</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3612,8 +3920,14 @@
       <c r="F12" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="16">
+      <c r="G12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3624,7 +3938,7 @@
         <v>-3.7492000000000001</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -3632,8 +3946,14 @@
       <c r="F13" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="16">
+      <c r="G13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3644,7 +3964,7 @@
         <v>-25.675599999999999</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -3652,8 +3972,14 @@
       <c r="F14" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="16">
+      <c r="G14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3664,7 +3990,7 @@
         <v>9.7497520000000009</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -3672,8 +3998,14 @@
       <c r="F15" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="16">
+      <c r="G15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3684,7 +4016,7 @@
         <v>28.08</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -3692,8 +4024,14 @@
       <c r="F16" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="16">
+      <c r="G16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3704,7 +4042,7 @@
         <v>55.27</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -3712,8 +4050,14 @@
       <c r="F17" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="16">
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3724,7 +4068,7 @@
         <v>57.552199999999999</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -3732,8 +4076,14 @@
       <c r="F18" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="16">
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3744,7 +4094,7 @@
         <v>77.5946</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -3752,8 +4102,14 @@
       <c r="F19" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="16">
+      <c r="G19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3764,7 +4120,7 @@
         <v>103.8198</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -3772,8 +4128,14 @@
       <c r="F20" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="16">
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3784,7 +4146,7 @@
         <v>139.6917</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -3792,8 +4154,14 @@
       <c r="F21" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="16">
+      <c r="G21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3804,13 +4172,19 @@
         <v>174.886</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>56</v>
+      </c>
+      <c r="G22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>